<commit_message>
transfer workspace from local to cloud
</commit_message>
<xml_diff>
--- a/第五章实验记录.xlsx
+++ b/第五章实验记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2a61c2c14f0bcf0/大论文/code/BatteryGPT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="11_AD4DA82427541F7ACA7EB8AA780A36766AE8DE1E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{676DDA58-4589-47FB-B55E-5D11FECCB9E5}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="11_AD4DA82427541F7ACA7EB8AA780A36766AE8DE1E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8823739-4342-4282-B2D8-BAD0AE19E88A}"/>
   <bookViews>
-    <workbookView xWindow="12285" yWindow="810" windowWidth="22755" windowHeight="19185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8850" yWindow="1695" windowWidth="20955" windowHeight="19185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>文件时间</t>
   </si>
@@ -70,6 +70,29 @@
   <si>
     <t>掩码模型，掩码数据，seq_len=24,label_len=12,pred_len=36。其余同上</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>b3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>非掩码模型，掩码数据，sl=24,ll=12,pl=48，关闭数据归一化。其余同上。效果不行</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>202403171514</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>b4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>关闭数据归一化，mmse损失。其余同b1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>202403181159</t>
   </si>
 </sst>
 </file>
@@ -461,7 +484,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A10" sqref="A10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -517,14 +540,26 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="8"/>
+      <c r="A5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="8"/>
+      <c r="A6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>

</xml_diff>